<commit_message>
完善php的正则函数 Signed-off-by: componey_qss <475185283@qq.com>
</commit_message>
<xml_diff>
--- a/php/php_数组和字符串.xlsx
+++ b/php/php_数组和字符串.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B5510F-2D44-486D-9E32-AB01D57D632F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A18D113-E88A-426A-8DA2-AF5455E28534}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,6 +59,22 @@
         </r>
       </text>
     </comment>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{21B53326-B17B-4794-947F-1D0A20145731}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">作者:
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C9" authorId="0" shapeId="0" xr:uid="{62E793C7-CB37-4953-821B-35AF1F28542A}">
       <text>
         <r>
@@ -96,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>preg_grep()</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -227,6 +243,14 @@
   <si>
     <t>同preg_replace
 mixed  $replacement=&gt;callable $callback   对匹配成功的字符串进行函数处理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string   $pattern              【必】查找规则
+string   $subject              【必】被查找的对象
+array    $matches            【选】返回匹配成功的字符串[0]以及子串[1][2]等  
+int        $flag                   【选】默认不返回字符串的位置。设PREG_OFFSET_CAPTURE则返
+int        $offset                【选】从offset开始匹配。offset可负数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -265,12 +289,36 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -337,16 +385,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -356,32 +401,65 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -692,30 +770,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F47091-127D-4D7D-9E03-778951866746}">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.75" style="9" customWidth="1"/>
-    <col min="2" max="2" width="15.75" style="5" customWidth="1"/>
-    <col min="3" max="3" width="10.625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="99.5" style="10" customWidth="1"/>
+    <col min="1" max="1" width="35.75" style="7" customWidth="1"/>
+    <col min="2" max="2" width="15.75" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="102.125" style="8" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>22</v>
       </c>
       <c r="E1" s="2"/>
@@ -737,16 +815,16 @@
       <c r="U1" s="2"/>
     </row>
     <row r="2" spans="1:21" ht="40.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="18" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="2"/>
@@ -768,16 +846,16 @@
       <c r="U2" s="2"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="2"/>
@@ -799,14 +877,14 @@
       <c r="U3" s="2"/>
     </row>
     <row r="4" spans="1:21" ht="101.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="2"/>
@@ -828,14 +906,14 @@
       <c r="U4" s="2"/>
     </row>
     <row r="5" spans="1:21" ht="40.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="2"/>
@@ -857,14 +935,14 @@
       <c r="U5" s="2"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -883,17 +961,19 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:21" ht="101.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -913,14 +993,14 @@
       <c r="U7" s="2"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -940,16 +1020,16 @@
       <c r="U8" s="2"/>
     </row>
     <row r="9" spans="1:21" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="2"/>
@@ -971,16 +1051,16 @@
       <c r="U9" s="2"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1000,14 +1080,14 @@
       <c r="U10" s="2"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1027,12 +1107,12 @@
       <c r="U11" s="2"/>
     </row>
     <row r="13" spans="1:21" ht="40.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1044,6 +1124,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>